<commit_message>
cambios antes de liberar
</commit_message>
<xml_diff>
--- a/Mundial/Presupuesto.xlsx
+++ b/Mundial/Presupuesto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>Concepto</t>
   </si>
@@ -152,6 +152,21 @@
   </si>
   <si>
     <t>Patos</t>
+  </si>
+  <si>
+    <t>Primer lugar</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Segundo Lugar</t>
+  </si>
+  <si>
+    <t>Tercer Lugar</t>
+  </si>
+  <si>
+    <t>Copa de Plata</t>
   </si>
 </sst>
 </file>
@@ -987,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,11 +1063,10 @@
         <v>1535</v>
       </c>
       <c r="E3" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1">
-        <f>D3*E3</f>
-        <v>49120</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1070,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F18" si="0">D4*E4</f>
+        <f t="shared" ref="F4:F23" si="0">D4*E4</f>
         <v>0</v>
       </c>
     </row>
@@ -1089,382 +1103,488 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F5" si="1">D5*E5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="1">
+        <v>60000</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1">
+        <v>30000</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1">
+        <v>30000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D10" s="2">
         <v>400</v>
       </c>
-      <c r="E6" s="2">
-        <f>B27</f>
+      <c r="E10" s="2">
+        <f>B34</f>
         <v>36</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>14400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2">
-        <v>480</v>
-      </c>
-      <c r="E7" s="2">
-        <f>B27</f>
-        <v>36</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>17280</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2">
-        <v>900</v>
-      </c>
-      <c r="E8" s="2">
-        <f>B27</f>
-        <v>36</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>32400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2">
-        <v>45</v>
-      </c>
-      <c r="E9" s="2">
-        <f>B27*4</f>
-        <v>144</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="2">
-        <v>160</v>
-      </c>
-      <c r="E10" s="2">
-        <f>B27*4</f>
-        <v>144</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>23040</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
+        <v>480</v>
+      </c>
+      <c r="E11" s="2">
+        <f>B34</f>
+        <v>36</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>17280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2">
+        <v>900</v>
+      </c>
+      <c r="E12" s="2">
+        <f>B34</f>
+        <v>36</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>32400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45</v>
+      </c>
+      <c r="E13" s="2">
+        <f>B34*4</f>
+        <v>144</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>160</v>
+      </c>
+      <c r="E14" s="2">
+        <f>B34*4</f>
+        <v>144</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>23040</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D15" s="2">
         <v>150</v>
       </c>
-      <c r="E11" s="2">
-        <f>B27*4</f>
+      <c r="E15" s="2">
+        <f>B34*4</f>
         <v>144</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>21600</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
         <v>100</v>
       </c>
-      <c r="E12" s="3">
-        <f>2*B27*4</f>
-        <v>288</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>28800</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
-        <v>900</v>
-      </c>
-      <c r="E13" s="3">
-        <f>4*2*B27/10</f>
-        <v>28.8</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>25920</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
-        <v>3000</v>
-      </c>
-      <c r="E14" s="3">
-        <f>B27*2*4/12</f>
-        <v>24</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>72000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
-        <v>150</v>
-      </c>
-      <c r="E15" s="3">
-        <f>B27*4*2</f>
-        <v>288</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>43200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1600</v>
-      </c>
       <c r="E16" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="3">
-        <v>2000</v>
+        <v>900</v>
       </c>
       <c r="E17" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3">
+        <v>3000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3">
+        <v>150</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1600</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2000</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D22" s="3">
         <v>1700</v>
       </c>
-      <c r="E18" s="3">
-        <f>B27</f>
+      <c r="E22" s="3">
         <v>36</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>61200</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="3">
+        <v>5500</v>
+      </c>
+      <c r="E23" s="3">
+        <v>40</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
         <f>8+12</f>
         <v>20</v>
       </c>
-      <c r="F19" s="4">
-        <f>D19*E19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4" t="s">
+      <c r="F26" s="4">
+        <f>D26*E26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
         <f>8+10</f>
         <v>18</v>
       </c>
-      <c r="F20" s="4">
-        <f>D20*E20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="F27" s="4">
+        <f>D27*E27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5">
         <v>100000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5">
         <v>250</v>
       </c>
-      <c r="E22" s="5">
-        <f>B27</f>
+      <c r="E29" s="5">
+        <f>B34</f>
         <v>36</v>
       </c>
-      <c r="F22" s="5">
-        <f>D22*E22</f>
+      <c r="F29" s="5">
+        <f>D29*E29</f>
         <v>9000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="B27">
+      <c r="B34">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B29">
-        <f>SUM(F2:F22)/B27</f>
-        <v>16990</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B36">
+        <f>SUM(F2:F29)/B34</f>
+        <v>22094.444444444445</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>40</v>
       </c>
-      <c r="B31">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B38">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
-      <c r="B32">
-        <f>B31*B27</f>
-        <v>756000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B39">
+        <f>B38*B34</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>42</v>
       </c>
-      <c r="B33">
-        <f>B32-SUM(F2:F22)</f>
-        <v>144360</v>
+      <c r="B40">
+        <f>B39-SUM(F2:F29)</f>
+        <v>104600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>